<commit_message>
Labs made before 17.09.2024
</commit_message>
<xml_diff>
--- a/Журнал.xlsx
+++ b/Журнал.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28105"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Sem5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E809453C-1410-4176-86F7-985F77585F04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{558F00D8-DA30-493F-A8B4-22F021910FD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="30">
   <si>
     <t>Валько</t>
   </si>
@@ -514,8 +514,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="AN1" sqref="AN1:AN3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="AN13" sqref="AN13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -659,24 +659,60 @@
       </c>
       <c r="T2" s="12"/>
       <c r="U2" s="12"/>
-      <c r="V2" s="1"/>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1"/>
-      <c r="AB2" s="1"/>
-      <c r="AC2" s="1"/>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1"/>
-      <c r="AH2" s="1"/>
-      <c r="AI2" s="1"/>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1"/>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="1"/>
+      <c r="V2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="AN2" s="12"/>
       <c r="AO2" s="12"/>
     </row>
@@ -738,24 +774,60 @@
       </c>
       <c r="T3" s="12"/>
       <c r="U3" s="12"/>
-      <c r="V3" s="5"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="5"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="5"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="5"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="5"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="5"/>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="5"/>
-      <c r="AI3" s="5"/>
-      <c r="AJ3" s="5"/>
-      <c r="AK3" s="5"/>
-      <c r="AL3" s="5"/>
-      <c r="AM3" s="5"/>
+      <c r="V3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="AB3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AC3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AE3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AF3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="AJ3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="AK3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="AL3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="AM3" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="AN3" s="12"/>
       <c r="AO3" s="12"/>
     </row>
@@ -783,24 +855,24 @@
       <c r="S4" s="8"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="1"/>
-      <c r="X4" s="1"/>
-      <c r="Y4" s="1"/>
-      <c r="Z4" s="1"/>
-      <c r="AA4" s="1"/>
-      <c r="AB4" s="1"/>
-      <c r="AC4" s="1"/>
-      <c r="AD4" s="1"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1"/>
-      <c r="AG4" s="1"/>
-      <c r="AH4" s="1"/>
-      <c r="AI4" s="1"/>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1"/>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="1"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+      <c r="AC4" s="8"/>
+      <c r="AD4" s="8"/>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8"/>
+      <c r="AG4" s="8"/>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="8"/>
+      <c r="AJ4" s="8"/>
+      <c r="AK4" s="8"/>
+      <c r="AL4" s="8"/>
+      <c r="AM4" s="8"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
     </row>
@@ -828,24 +900,24 @@
       <c r="S5" s="8"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-      <c r="X5" s="1"/>
-      <c r="Y5" s="1"/>
-      <c r="Z5" s="1"/>
-      <c r="AA5" s="1"/>
-      <c r="AB5" s="1"/>
-      <c r="AC5" s="1"/>
-      <c r="AD5" s="1"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
-      <c r="AH5" s="1"/>
-      <c r="AI5" s="1"/>
-      <c r="AJ5" s="1"/>
-      <c r="AK5" s="1"/>
-      <c r="AL5" s="1"/>
-      <c r="AM5" s="1"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="8"/>
+      <c r="X5" s="8"/>
+      <c r="Y5" s="8"/>
+      <c r="Z5" s="8"/>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="8"/>
+      <c r="AD5" s="8"/>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8"/>
+      <c r="AG5" s="8"/>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="8"/>
+      <c r="AJ5" s="8"/>
+      <c r="AK5" s="8"/>
+      <c r="AL5" s="8"/>
+      <c r="AM5" s="8"/>
       <c r="AN5" s="1"/>
       <c r="AO5" s="1"/>
     </row>
@@ -873,24 +945,24 @@
       <c r="S6" s="8"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="1"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="1"/>
-      <c r="AB6" s="1"/>
-      <c r="AC6" s="1"/>
-      <c r="AD6" s="1"/>
-      <c r="AE6" s="1"/>
-      <c r="AF6" s="1"/>
-      <c r="AG6" s="1"/>
-      <c r="AH6" s="1"/>
-      <c r="AI6" s="1"/>
-      <c r="AJ6" s="1"/>
-      <c r="AK6" s="1"/>
-      <c r="AL6" s="1"/>
-      <c r="AM6" s="1"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8"/>
+      <c r="AC6" s="8"/>
+      <c r="AD6" s="8"/>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8"/>
+      <c r="AG6" s="8"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
+      <c r="AK6" s="8"/>
+      <c r="AL6" s="8"/>
+      <c r="AM6" s="8"/>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
     </row>
@@ -918,24 +990,24 @@
       <c r="S7" s="8"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-      <c r="Y7" s="1"/>
-      <c r="Z7" s="1"/>
-      <c r="AA7" s="1"/>
-      <c r="AB7" s="1"/>
-      <c r="AC7" s="1"/>
-      <c r="AD7" s="1"/>
-      <c r="AE7" s="1"/>
-      <c r="AF7" s="1"/>
-      <c r="AG7" s="1"/>
-      <c r="AH7" s="1"/>
-      <c r="AI7" s="1"/>
-      <c r="AJ7" s="1"/>
-      <c r="AK7" s="1"/>
-      <c r="AL7" s="1"/>
-      <c r="AM7" s="1"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8"/>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8"/>
+      <c r="AC7" s="8"/>
+      <c r="AD7" s="8"/>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8"/>
+      <c r="AG7" s="8"/>
+      <c r="AH7" s="8"/>
+      <c r="AI7" s="8"/>
+      <c r="AJ7" s="8"/>
+      <c r="AK7" s="8"/>
+      <c r="AL7" s="8"/>
+      <c r="AM7" s="8"/>
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
     </row>
@@ -963,24 +1035,24 @@
       <c r="S8" s="8"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="1"/>
-      <c r="AC8" s="1"/>
-      <c r="AD8" s="1"/>
-      <c r="AE8" s="1"/>
-      <c r="AF8" s="1"/>
-      <c r="AG8" s="1"/>
-      <c r="AH8" s="1"/>
-      <c r="AI8" s="1"/>
-      <c r="AJ8" s="1"/>
-      <c r="AK8" s="1"/>
-      <c r="AL8" s="1"/>
-      <c r="AM8" s="1"/>
+      <c r="V8" s="8"/>
+      <c r="W8" s="8"/>
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8"/>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="8"/>
+      <c r="AD8" s="8"/>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8"/>
+      <c r="AG8" s="8"/>
+      <c r="AH8" s="8"/>
+      <c r="AI8" s="8"/>
+      <c r="AJ8" s="8"/>
+      <c r="AK8" s="8"/>
+      <c r="AL8" s="8"/>
+      <c r="AM8" s="8"/>
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
     </row>
@@ -1008,26 +1080,28 @@
       <c r="S9" s="8"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
-      <c r="AC9" s="1"/>
-      <c r="AD9" s="1"/>
-      <c r="AE9" s="1"/>
-      <c r="AF9" s="1"/>
-      <c r="AG9" s="1"/>
-      <c r="AH9" s="1"/>
-      <c r="AI9" s="1"/>
-      <c r="AJ9" s="1"/>
-      <c r="AK9" s="1"/>
-      <c r="AL9" s="1"/>
-      <c r="AM9" s="1"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="8"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="8"/>
+      <c r="AG9" s="10"/>
+      <c r="AH9" s="8"/>
+      <c r="AI9" s="10"/>
+      <c r="AJ9" s="8"/>
+      <c r="AK9" s="8"/>
+      <c r="AL9" s="8"/>
+      <c r="AM9" s="8"/>
       <c r="AN9" s="1"/>
-      <c r="AO9" s="1"/>
+      <c r="AO9" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:41" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
@@ -1053,24 +1127,24 @@
       <c r="S10" s="8"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
-      <c r="V10" s="1"/>
-      <c r="W10" s="1"/>
-      <c r="X10" s="1"/>
-      <c r="Y10" s="1"/>
-      <c r="Z10" s="1"/>
-      <c r="AA10" s="1"/>
-      <c r="AB10" s="1"/>
-      <c r="AC10" s="1"/>
-      <c r="AD10" s="1"/>
-      <c r="AE10" s="1"/>
-      <c r="AF10" s="1"/>
-      <c r="AG10" s="1"/>
-      <c r="AH10" s="1"/>
-      <c r="AI10" s="1"/>
-      <c r="AJ10" s="1"/>
-      <c r="AK10" s="1"/>
-      <c r="AL10" s="1"/>
-      <c r="AM10" s="1"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8"/>
+      <c r="AG10" s="8"/>
+      <c r="AH10" s="8"/>
+      <c r="AI10" s="8"/>
+      <c r="AJ10" s="8"/>
+      <c r="AK10" s="8"/>
+      <c r="AL10" s="8"/>
+      <c r="AM10" s="8"/>
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
     </row>
@@ -1098,24 +1172,24 @@
       <c r="S11" s="8"/>
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="1"/>
-      <c r="X11" s="1"/>
-      <c r="Y11" s="1"/>
-      <c r="Z11" s="1"/>
-      <c r="AA11" s="1"/>
-      <c r="AB11" s="1"/>
-      <c r="AC11" s="1"/>
-      <c r="AD11" s="1"/>
-      <c r="AE11" s="1"/>
-      <c r="AF11" s="1"/>
-      <c r="AG11" s="1"/>
-      <c r="AH11" s="1"/>
-      <c r="AI11" s="1"/>
-      <c r="AJ11" s="1"/>
-      <c r="AK11" s="1"/>
-      <c r="AL11" s="1"/>
-      <c r="AM11" s="1"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="8"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="8"/>
+      <c r="AD11" s="8"/>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="8"/>
+      <c r="AG11" s="8"/>
+      <c r="AH11" s="8"/>
+      <c r="AI11" s="8"/>
+      <c r="AJ11" s="8"/>
+      <c r="AK11" s="8"/>
+      <c r="AL11" s="8"/>
+      <c r="AM11" s="8"/>
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
     </row>
@@ -1145,26 +1219,28 @@
       <c r="U12" s="1">
         <v>2</v>
       </c>
-      <c r="V12" s="1"/>
-      <c r="W12" s="1"/>
-      <c r="X12" s="1"/>
-      <c r="Y12" s="1"/>
-      <c r="Z12" s="1"/>
-      <c r="AA12" s="1"/>
-      <c r="AB12" s="1"/>
-      <c r="AC12" s="1"/>
-      <c r="AD12" s="1"/>
-      <c r="AE12" s="1"/>
-      <c r="AF12" s="1"/>
-      <c r="AG12" s="1"/>
-      <c r="AH12" s="1"/>
-      <c r="AI12" s="1"/>
-      <c r="AJ12" s="1"/>
-      <c r="AK12" s="1"/>
-      <c r="AL12" s="1"/>
-      <c r="AM12" s="1"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="8"/>
+      <c r="AC12" s="8"/>
+      <c r="AD12" s="8"/>
+      <c r="AE12" s="8"/>
+      <c r="AF12" s="8"/>
+      <c r="AG12" s="10"/>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="10"/>
+      <c r="AJ12" s="8"/>
+      <c r="AK12" s="8"/>
+      <c r="AL12" s="8"/>
+      <c r="AM12" s="8"/>
       <c r="AN12" s="1"/>
-      <c r="AO12" s="1"/>
+      <c r="AO12" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="13" spans="1:41" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
@@ -1192,26 +1268,28 @@
       <c r="U13" s="1">
         <v>4</v>
       </c>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-      <c r="X13" s="1"/>
-      <c r="Y13" s="1"/>
-      <c r="Z13" s="1"/>
-      <c r="AA13" s="1"/>
-      <c r="AB13" s="1"/>
-      <c r="AC13" s="1"/>
-      <c r="AD13" s="1"/>
-      <c r="AE13" s="1"/>
-      <c r="AF13" s="1"/>
-      <c r="AG13" s="1"/>
-      <c r="AH13" s="1"/>
-      <c r="AI13" s="1"/>
-      <c r="AJ13" s="1"/>
-      <c r="AK13" s="1"/>
-      <c r="AL13" s="1"/>
-      <c r="AM13" s="1"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
+      <c r="AA13" s="8"/>
+      <c r="AB13" s="8"/>
+      <c r="AC13" s="8"/>
+      <c r="AD13" s="8"/>
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="8"/>
+      <c r="AG13" s="8"/>
+      <c r="AH13" s="8"/>
+      <c r="AI13" s="10"/>
+      <c r="AJ13" s="8"/>
+      <c r="AK13" s="8"/>
+      <c r="AL13" s="8"/>
+      <c r="AM13" s="8"/>
       <c r="AN13" s="1"/>
-      <c r="AO13" s="1"/>
+      <c r="AO13" s="1">
+        <v>8</v>
+      </c>
     </row>
     <row r="14" spans="1:41" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
@@ -1237,24 +1315,24 @@
       <c r="S14" s="8"/>
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
-      <c r="V14" s="1"/>
-      <c r="W14" s="1"/>
-      <c r="X14" s="1"/>
-      <c r="Y14" s="1"/>
-      <c r="Z14" s="1"/>
-      <c r="AA14" s="1"/>
-      <c r="AB14" s="1"/>
-      <c r="AC14" s="1"/>
-      <c r="AD14" s="1"/>
-      <c r="AE14" s="1"/>
-      <c r="AF14" s="1"/>
-      <c r="AG14" s="1"/>
-      <c r="AH14" s="1"/>
-      <c r="AI14" s="1"/>
-      <c r="AJ14" s="1"/>
-      <c r="AK14" s="1"/>
-      <c r="AL14" s="1"/>
-      <c r="AM14" s="1"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8"/>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="8"/>
+      <c r="AD14" s="8"/>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8"/>
+      <c r="AG14" s="8"/>
+      <c r="AH14" s="8"/>
+      <c r="AI14" s="8"/>
+      <c r="AJ14" s="8"/>
+      <c r="AK14" s="8"/>
+      <c r="AL14" s="8"/>
+      <c r="AM14" s="8"/>
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
     </row>
@@ -1282,24 +1360,24 @@
       <c r="S15" s="8"/>
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-      <c r="X15" s="1"/>
-      <c r="Y15" s="1"/>
-      <c r="Z15" s="1"/>
-      <c r="AA15" s="1"/>
-      <c r="AB15" s="1"/>
-      <c r="AC15" s="1"/>
-      <c r="AD15" s="1"/>
-      <c r="AE15" s="1"/>
-      <c r="AF15" s="1"/>
-      <c r="AG15" s="1"/>
-      <c r="AH15" s="1"/>
-      <c r="AI15" s="1"/>
-      <c r="AJ15" s="1"/>
-      <c r="AK15" s="1"/>
-      <c r="AL15" s="1"/>
-      <c r="AM15" s="1"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8"/>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8"/>
+      <c r="AA15" s="8"/>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="8"/>
+      <c r="AD15" s="8"/>
+      <c r="AE15" s="8"/>
+      <c r="AF15" s="8"/>
+      <c r="AG15" s="8"/>
+      <c r="AH15" s="8"/>
+      <c r="AI15" s="8"/>
+      <c r="AJ15" s="8"/>
+      <c r="AK15" s="8"/>
+      <c r="AL15" s="8"/>
+      <c r="AM15" s="8"/>
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
     </row>
@@ -1327,24 +1405,24 @@
       <c r="S16" s="8"/>
       <c r="T16" s="1"/>
       <c r="U16" s="1"/>
-      <c r="V16" s="1"/>
-      <c r="W16" s="1"/>
-      <c r="X16" s="1"/>
-      <c r="Y16" s="1"/>
-      <c r="Z16" s="1"/>
-      <c r="AA16" s="1"/>
-      <c r="AB16" s="1"/>
-      <c r="AC16" s="1"/>
-      <c r="AD16" s="1"/>
-      <c r="AE16" s="1"/>
-      <c r="AF16" s="1"/>
-      <c r="AG16" s="1"/>
-      <c r="AH16" s="1"/>
-      <c r="AI16" s="1"/>
-      <c r="AJ16" s="1"/>
-      <c r="AK16" s="1"/>
-      <c r="AL16" s="1"/>
-      <c r="AM16" s="1"/>
+      <c r="V16" s="8"/>
+      <c r="W16" s="8"/>
+      <c r="X16" s="8"/>
+      <c r="Y16" s="8"/>
+      <c r="Z16" s="8"/>
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8"/>
+      <c r="AH16" s="8"/>
+      <c r="AI16" s="8"/>
+      <c r="AJ16" s="8"/>
+      <c r="AK16" s="8"/>
+      <c r="AL16" s="8"/>
+      <c r="AM16" s="8"/>
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
     </row>
@@ -1372,24 +1450,24 @@
       <c r="S17" s="8"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
-      <c r="V17" s="1"/>
-      <c r="W17" s="1"/>
-      <c r="X17" s="1"/>
-      <c r="Y17" s="1"/>
-      <c r="Z17" s="1"/>
-      <c r="AA17" s="1"/>
-      <c r="AB17" s="1"/>
-      <c r="AC17" s="1"/>
-      <c r="AD17" s="1"/>
-      <c r="AE17" s="1"/>
-      <c r="AF17" s="1"/>
-      <c r="AG17" s="1"/>
-      <c r="AH17" s="1"/>
-      <c r="AI17" s="1"/>
-      <c r="AJ17" s="1"/>
-      <c r="AK17" s="1"/>
-      <c r="AL17" s="1"/>
-      <c r="AM17" s="1"/>
+      <c r="V17" s="8"/>
+      <c r="W17" s="8"/>
+      <c r="X17" s="8"/>
+      <c r="Y17" s="8"/>
+      <c r="Z17" s="8"/>
+      <c r="AA17" s="8"/>
+      <c r="AB17" s="8"/>
+      <c r="AC17" s="8"/>
+      <c r="AD17" s="8"/>
+      <c r="AE17" s="8"/>
+      <c r="AF17" s="8"/>
+      <c r="AG17" s="8"/>
+      <c r="AH17" s="8"/>
+      <c r="AI17" s="8"/>
+      <c r="AJ17" s="8"/>
+      <c r="AK17" s="8"/>
+      <c r="AL17" s="8"/>
+      <c r="AM17" s="8"/>
       <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
     </row>
@@ -1417,29 +1495,37 @@
       <c r="S18" s="8"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
-      <c r="V18" s="1"/>
-      <c r="W18" s="1"/>
-      <c r="X18" s="1"/>
-      <c r="Y18" s="1"/>
-      <c r="Z18" s="1"/>
-      <c r="AA18" s="1"/>
-      <c r="AB18" s="1"/>
-      <c r="AC18" s="1"/>
-      <c r="AD18" s="1"/>
-      <c r="AE18" s="1"/>
-      <c r="AF18" s="1"/>
-      <c r="AG18" s="1"/>
-      <c r="AH18" s="1"/>
-      <c r="AI18" s="1"/>
-      <c r="AJ18" s="1"/>
-      <c r="AK18" s="1"/>
-      <c r="AL18" s="1"/>
-      <c r="AM18" s="1"/>
+      <c r="V18" s="8"/>
+      <c r="W18" s="8"/>
+      <c r="X18" s="8"/>
+      <c r="Y18" s="8"/>
+      <c r="Z18" s="8"/>
+      <c r="AA18" s="8"/>
+      <c r="AB18" s="8"/>
+      <c r="AC18" s="8"/>
+      <c r="AD18" s="8"/>
+      <c r="AE18" s="8"/>
+      <c r="AF18" s="8"/>
+      <c r="AG18" s="8"/>
+      <c r="AH18" s="8"/>
+      <c r="AI18" s="8"/>
+      <c r="AJ18" s="8"/>
+      <c r="AK18" s="8"/>
+      <c r="AL18" s="8"/>
+      <c r="AM18" s="8"/>
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:O1"/>
     <mergeCell ref="AJ1:AM1"/>
     <mergeCell ref="AO1:AO3"/>
     <mergeCell ref="AN1:AN3"/>
@@ -1448,14 +1534,6 @@
     <mergeCell ref="AB1:AD1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AG1:AI1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Labs made before 28.09.2024
</commit_message>
<xml_diff>
--- a/Журнал.xlsx
+++ b/Журнал.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28125"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\Sem5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD95088-35E7-4CB8-8F49-1F9A9FD8412B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{259BE3BD-D414-4834-9847-005CA1251CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="30">
   <si>
     <t>Валько</t>
   </si>
@@ -176,7 +176,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -199,11 +199,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -223,6 +260,8 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -232,9 +271,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -515,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI18"/>
+  <dimension ref="A1:CC18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T4" workbookViewId="0">
-      <selection activeCell="AY7" sqref="AY7"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="BL5" sqref="BL5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,118 +577,154 @@
     <col min="52" max="52" width="3.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="11">
+      <c r="B1" s="13">
         <v>45537</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="11">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="13">
         <v>45538</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="11">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="13">
         <v>45539</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="11">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="13">
         <v>45540</v>
       </c>
-      <c r="L1" s="13"/>
-      <c r="M1" s="11">
+      <c r="L1" s="15"/>
+      <c r="M1" s="13">
         <v>45541</v>
       </c>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="11">
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="13">
         <v>45542</v>
       </c>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="12" t="s">
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="11">
+      <c r="V1" s="13">
         <v>45544</v>
       </c>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="11">
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="13">
         <v>45545</v>
       </c>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="11">
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+      <c r="AB1" s="13">
         <v>45546</v>
       </c>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="11">
+      <c r="AC1" s="15"/>
+      <c r="AD1" s="15"/>
+      <c r="AE1" s="13">
         <v>45547</v>
       </c>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="11">
+      <c r="AF1" s="15"/>
+      <c r="AG1" s="13">
         <v>45548</v>
       </c>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="11">
+      <c r="AH1" s="15"/>
+      <c r="AI1" s="15"/>
+      <c r="AJ1" s="13">
         <v>45549</v>
       </c>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11"/>
-      <c r="AM1" s="11"/>
-      <c r="AN1" s="12" t="s">
+      <c r="AK1" s="13"/>
+      <c r="AL1" s="13"/>
+      <c r="AM1" s="13"/>
+      <c r="AN1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="AO1" s="12" t="s">
+      <c r="AO1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="AP1" s="11">
-        <v>45537</v>
-      </c>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="11">
-        <v>45538</v>
-      </c>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="11">
-        <v>45539</v>
-      </c>
-      <c r="AW1" s="13"/>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="11">
-        <v>45540</v>
-      </c>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="11">
-        <v>45541</v>
-      </c>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="11">
-        <v>45542</v>
-      </c>
-      <c r="BE1" s="11"/>
-      <c r="BF1" s="11"/>
-      <c r="BG1" s="11"/>
-      <c r="BH1" s="12" t="s">
+      <c r="AP1" s="13">
+        <v>45551</v>
+      </c>
+      <c r="AQ1" s="15"/>
+      <c r="AR1" s="15"/>
+      <c r="AS1" s="13">
+        <v>45552</v>
+      </c>
+      <c r="AT1" s="15"/>
+      <c r="AU1" s="15"/>
+      <c r="AV1" s="13">
+        <v>45553</v>
+      </c>
+      <c r="AW1" s="15"/>
+      <c r="AX1" s="15"/>
+      <c r="AY1" s="13">
+        <v>45554</v>
+      </c>
+      <c r="AZ1" s="15"/>
+      <c r="BA1" s="13">
+        <v>45555</v>
+      </c>
+      <c r="BB1" s="15"/>
+      <c r="BC1" s="15"/>
+      <c r="BD1" s="13">
+        <v>45556</v>
+      </c>
+      <c r="BE1" s="13"/>
+      <c r="BF1" s="13"/>
+      <c r="BG1" s="13"/>
+      <c r="BH1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="BI1" s="12" t="s">
+      <c r="BI1" s="14" t="s">
         <v>21</v>
       </c>
+      <c r="BJ1" s="13">
+        <v>45558</v>
+      </c>
+      <c r="BK1" s="15"/>
+      <c r="BL1" s="15"/>
+      <c r="BM1" s="13">
+        <v>45559</v>
+      </c>
+      <c r="BN1" s="15"/>
+      <c r="BO1" s="15"/>
+      <c r="BP1" s="13">
+        <v>45560</v>
+      </c>
+      <c r="BQ1" s="15"/>
+      <c r="BR1" s="15"/>
+      <c r="BS1" s="16">
+        <v>45561</v>
+      </c>
+      <c r="BT1" s="17"/>
+      <c r="BU1" s="18"/>
+      <c r="BV1" s="13">
+        <v>45562</v>
+      </c>
+      <c r="BW1" s="15"/>
+      <c r="BX1" s="15"/>
+      <c r="BY1" s="16">
+        <v>45563</v>
+      </c>
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="18"/>
+      <c r="CB1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="CC1" s="14" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>19</v>
@@ -698,8 +780,8 @@
       <c r="S2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
+      <c r="T2" s="14"/>
+      <c r="U2" s="14"/>
       <c r="V2" s="2" t="s">
         <v>19</v>
       </c>
@@ -754,8 +836,8 @@
       <c r="AM2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AN2" s="12"/>
-      <c r="AO2" s="12"/>
+      <c r="AN2" s="14"/>
+      <c r="AO2" s="14"/>
       <c r="AP2" s="2" t="s">
         <v>19</v>
       </c>
@@ -810,10 +892,66 @@
       <c r="BG2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="BH2" s="12"/>
-      <c r="BI2" s="12"/>
+      <c r="BH2" s="14"/>
+      <c r="BI2" s="14"/>
+      <c r="BJ2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="BK2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="BL2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="BM2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="BN2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BO2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BP2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BQ2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="BR2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BS2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BT2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="BU2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BV2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="BW2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BX2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="BY2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="BZ2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="CA2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="CB2" s="14"/>
+      <c r="CC2" s="14"/>
     </row>
-    <row r="3" spans="1:61" s="6" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:81" s="6" customFormat="1" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="5" t="s">
         <v>15</v>
@@ -869,8 +1007,8 @@
       <c r="S3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="T3" s="12"/>
-      <c r="U3" s="12"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
       <c r="V3" s="5" t="s">
         <v>15</v>
       </c>
@@ -925,8 +1063,8 @@
       <c r="AM3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="AN3" s="12"/>
-      <c r="AO3" s="12"/>
+      <c r="AN3" s="14"/>
+      <c r="AO3" s="14"/>
       <c r="AP3" s="5" t="s">
         <v>15</v>
       </c>
@@ -981,10 +1119,66 @@
       <c r="BG3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="BH3" s="12"/>
-      <c r="BI3" s="12"/>
+      <c r="BH3" s="14"/>
+      <c r="BI3" s="14"/>
+      <c r="BJ3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="BK3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="BL3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="BM3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="BN3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="BO3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="BP3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="BQ3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="BR3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="BS3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="BT3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="BU3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="BV3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="BW3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="BX3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="BY3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="BZ3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="CA3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="CB3" s="14"/>
+      <c r="CC3" s="14"/>
     </row>
-    <row r="4" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -1028,14 +1222,33 @@
       <c r="AM4" s="8"/>
       <c r="AN4" s="1"/>
       <c r="AP4" s="8"/>
-      <c r="AQ4" s="15"/>
-      <c r="AR4" s="15"/>
-      <c r="AS4" s="15"/>
-      <c r="AT4" s="15"/>
-      <c r="AU4" s="15"/>
-      <c r="AV4" s="15"/>
+      <c r="AQ4" s="12"/>
+      <c r="AR4" s="12"/>
+      <c r="AS4" s="12"/>
+      <c r="AT4" s="12"/>
+      <c r="AU4" s="12"/>
+      <c r="AV4" s="12"/>
+      <c r="BJ4" s="19"/>
+      <c r="BK4" s="19"/>
+      <c r="BL4" s="19"/>
+      <c r="BM4" s="19"/>
+      <c r="BN4" s="19"/>
+      <c r="BO4" s="19"/>
+      <c r="BP4" s="19"/>
+      <c r="BQ4" s="19"/>
+      <c r="BR4" s="19"/>
+      <c r="BS4" s="19"/>
+      <c r="BT4" s="19"/>
+      <c r="BU4" s="19"/>
+      <c r="BV4" s="19"/>
+      <c r="BW4" s="19"/>
+      <c r="BX4" s="19"/>
+      <c r="BY4" s="19"/>
+      <c r="BZ4" s="19"/>
+      <c r="CA4" s="19"/>
+      <c r="CB4" s="19"/>
     </row>
-    <row r="5" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
@@ -1079,14 +1292,33 @@
       <c r="AM5" s="8"/>
       <c r="AN5" s="1"/>
       <c r="AP5" s="8"/>
-      <c r="AQ5" s="15"/>
-      <c r="AR5" s="15"/>
-      <c r="AS5" s="15"/>
-      <c r="AT5" s="15"/>
-      <c r="AU5" s="15"/>
-      <c r="AV5" s="15"/>
+      <c r="AQ5" s="12"/>
+      <c r="AR5" s="12"/>
+      <c r="AS5" s="12"/>
+      <c r="AT5" s="12"/>
+      <c r="AU5" s="12"/>
+      <c r="AV5" s="12"/>
+      <c r="BJ5" s="19"/>
+      <c r="BK5" s="19"/>
+      <c r="BL5" s="19"/>
+      <c r="BM5" s="19"/>
+      <c r="BN5" s="19"/>
+      <c r="BO5" s="19"/>
+      <c r="BP5" s="19"/>
+      <c r="BQ5" s="19"/>
+      <c r="BR5" s="19"/>
+      <c r="BS5" s="19"/>
+      <c r="BT5" s="19"/>
+      <c r="BU5" s="19"/>
+      <c r="BV5" s="19"/>
+      <c r="BW5" s="19"/>
+      <c r="BX5" s="19"/>
+      <c r="BY5" s="19"/>
+      <c r="BZ5" s="19"/>
+      <c r="CA5" s="19"/>
+      <c r="CB5" s="19"/>
     </row>
-    <row r="6" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="9" t="s">
         <v>2</v>
       </c>
@@ -1130,14 +1362,33 @@
       <c r="AM6" s="8"/>
       <c r="AN6" s="1"/>
       <c r="AP6" s="8"/>
-      <c r="AQ6" s="15"/>
-      <c r="AR6" s="15"/>
-      <c r="AS6" s="15"/>
-      <c r="AT6" s="15"/>
-      <c r="AU6" s="15"/>
-      <c r="AV6" s="15"/>
+      <c r="AQ6" s="12"/>
+      <c r="AR6" s="12"/>
+      <c r="AS6" s="12"/>
+      <c r="AT6" s="12"/>
+      <c r="AU6" s="12"/>
+      <c r="AV6" s="12"/>
+      <c r="BJ6" s="19"/>
+      <c r="BK6" s="19"/>
+      <c r="BL6" s="19"/>
+      <c r="BM6" s="19"/>
+      <c r="BN6" s="19"/>
+      <c r="BO6" s="19"/>
+      <c r="BP6" s="19"/>
+      <c r="BQ6" s="19"/>
+      <c r="BR6" s="19"/>
+      <c r="BS6" s="19"/>
+      <c r="BT6" s="19"/>
+      <c r="BU6" s="19"/>
+      <c r="BV6" s="19"/>
+      <c r="BW6" s="19"/>
+      <c r="BX6" s="19"/>
+      <c r="BY6" s="19"/>
+      <c r="BZ6" s="19"/>
+      <c r="CA6" s="19"/>
+      <c r="CB6" s="19"/>
     </row>
-    <row r="7" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>3</v>
       </c>
@@ -1181,15 +1432,34 @@
       <c r="AM7" s="8"/>
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
-      <c r="AP7" s="15"/>
-      <c r="AQ7" s="15"/>
-      <c r="AR7" s="15"/>
-      <c r="AS7" s="15"/>
-      <c r="AT7" s="15"/>
-      <c r="AU7" s="15"/>
-      <c r="AV7" s="15"/>
+      <c r="AP7" s="12"/>
+      <c r="AQ7" s="12"/>
+      <c r="AR7" s="12"/>
+      <c r="AS7" s="12"/>
+      <c r="AT7" s="12"/>
+      <c r="AU7" s="12"/>
+      <c r="AV7" s="12"/>
+      <c r="BJ7" s="19"/>
+      <c r="BK7" s="19"/>
+      <c r="BL7" s="19"/>
+      <c r="BM7" s="19"/>
+      <c r="BN7" s="19"/>
+      <c r="BO7" s="19"/>
+      <c r="BP7" s="19"/>
+      <c r="BQ7" s="19"/>
+      <c r="BR7" s="19"/>
+      <c r="BS7" s="19"/>
+      <c r="BT7" s="19"/>
+      <c r="BU7" s="19"/>
+      <c r="BV7" s="19"/>
+      <c r="BW7" s="19"/>
+      <c r="BX7" s="19"/>
+      <c r="BY7" s="19"/>
+      <c r="BZ7" s="19"/>
+      <c r="CA7" s="19"/>
+      <c r="CB7" s="19"/>
     </row>
-    <row r="8" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
@@ -1233,15 +1503,34 @@
       <c r="AM8" s="8"/>
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
-      <c r="AP8" s="15"/>
-      <c r="AQ8" s="15"/>
-      <c r="AR8" s="15"/>
-      <c r="AS8" s="15"/>
-      <c r="AT8" s="15"/>
-      <c r="AU8" s="15"/>
-      <c r="AV8" s="15"/>
+      <c r="AP8" s="12"/>
+      <c r="AQ8" s="12"/>
+      <c r="AR8" s="12"/>
+      <c r="AS8" s="12"/>
+      <c r="AT8" s="12"/>
+      <c r="AU8" s="12"/>
+      <c r="AV8" s="12"/>
+      <c r="BJ8" s="19"/>
+      <c r="BK8" s="19"/>
+      <c r="BL8" s="19"/>
+      <c r="BM8" s="19"/>
+      <c r="BN8" s="19"/>
+      <c r="BO8" s="19"/>
+      <c r="BP8" s="19"/>
+      <c r="BQ8" s="19"/>
+      <c r="BR8" s="19"/>
+      <c r="BS8" s="19"/>
+      <c r="BT8" s="19"/>
+      <c r="BU8" s="19"/>
+      <c r="BV8" s="19"/>
+      <c r="BW8" s="19"/>
+      <c r="BX8" s="19"/>
+      <c r="BY8" s="19"/>
+      <c r="BZ8" s="19"/>
+      <c r="CA8" s="19"/>
+      <c r="CB8" s="19"/>
     </row>
-    <row r="9" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="7" t="s">
         <v>5</v>
       </c>
@@ -1287,15 +1576,33 @@
       <c r="AO9" s="1">
         <v>6</v>
       </c>
-      <c r="AP9" s="14"/>
-      <c r="AQ9" s="15"/>
-      <c r="AR9" s="16"/>
-      <c r="AS9" s="14"/>
-      <c r="AT9" s="15"/>
-      <c r="AU9" s="15"/>
-      <c r="AV9" s="15"/>
+      <c r="AP9" s="11"/>
+      <c r="AQ9" s="12"/>
+      <c r="AS9" s="11"/>
+      <c r="AT9" s="12"/>
+      <c r="AU9" s="12"/>
+      <c r="AV9" s="12"/>
+      <c r="BJ9" s="19"/>
+      <c r="BK9" s="19"/>
+      <c r="BL9" s="19"/>
+      <c r="BM9" s="19"/>
+      <c r="BN9" s="19"/>
+      <c r="BO9" s="19"/>
+      <c r="BP9" s="19"/>
+      <c r="BQ9" s="19"/>
+      <c r="BR9" s="19"/>
+      <c r="BS9" s="19"/>
+      <c r="BT9" s="19"/>
+      <c r="BU9" s="19"/>
+      <c r="BV9" s="19"/>
+      <c r="BW9" s="19"/>
+      <c r="BX9" s="19"/>
+      <c r="BY9" s="19"/>
+      <c r="BZ9" s="19"/>
+      <c r="CA9" s="19"/>
+      <c r="CB9" s="19"/>
     </row>
-    <row r="10" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
@@ -1339,15 +1646,34 @@
       <c r="AM10" s="8"/>
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
-      <c r="AP10" s="15"/>
-      <c r="AQ10" s="15"/>
-      <c r="AR10" s="15"/>
-      <c r="AS10" s="15"/>
-      <c r="AT10" s="15"/>
-      <c r="AU10" s="15"/>
-      <c r="AV10" s="15"/>
+      <c r="AP10" s="12"/>
+      <c r="AQ10" s="12"/>
+      <c r="AR10" s="12"/>
+      <c r="AS10" s="12"/>
+      <c r="AT10" s="12"/>
+      <c r="AU10" s="12"/>
+      <c r="AV10" s="12"/>
+      <c r="BJ10" s="19"/>
+      <c r="BK10" s="19"/>
+      <c r="BL10" s="19"/>
+      <c r="BM10" s="19"/>
+      <c r="BN10" s="19"/>
+      <c r="BO10" s="19"/>
+      <c r="BP10" s="19"/>
+      <c r="BQ10" s="19"/>
+      <c r="BR10" s="19"/>
+      <c r="BS10" s="19"/>
+      <c r="BT10" s="19"/>
+      <c r="BU10" s="19"/>
+      <c r="BV10" s="19"/>
+      <c r="BW10" s="19"/>
+      <c r="BX10" s="19"/>
+      <c r="BY10" s="19"/>
+      <c r="BZ10" s="19"/>
+      <c r="CA10" s="19"/>
+      <c r="CB10" s="19"/>
     </row>
-    <row r="11" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
         <v>7</v>
       </c>
@@ -1391,15 +1717,34 @@
       <c r="AM11" s="8"/>
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
-      <c r="AP11" s="15"/>
-      <c r="AQ11" s="15"/>
-      <c r="AR11" s="15"/>
-      <c r="AS11" s="15"/>
-      <c r="AT11" s="15"/>
-      <c r="AU11" s="15"/>
-      <c r="AV11" s="15"/>
+      <c r="AP11" s="12"/>
+      <c r="AQ11" s="12"/>
+      <c r="AR11" s="12"/>
+      <c r="AS11" s="12"/>
+      <c r="AT11" s="12"/>
+      <c r="AU11" s="12"/>
+      <c r="AV11" s="12"/>
+      <c r="BJ11" s="19"/>
+      <c r="BK11" s="19"/>
+      <c r="BL11" s="19"/>
+      <c r="BM11" s="19"/>
+      <c r="BN11" s="19"/>
+      <c r="BO11" s="19"/>
+      <c r="BP11" s="19"/>
+      <c r="BQ11" s="19"/>
+      <c r="BR11" s="19"/>
+      <c r="BS11" s="19"/>
+      <c r="BT11" s="19"/>
+      <c r="BU11" s="19"/>
+      <c r="BV11" s="19"/>
+      <c r="BW11" s="19"/>
+      <c r="BX11" s="19"/>
+      <c r="BY11" s="19"/>
+      <c r="BZ11" s="19"/>
+      <c r="CA11" s="19"/>
+      <c r="CB11" s="19"/>
     </row>
-    <row r="12" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>8</v>
       </c>
@@ -1447,15 +1792,34 @@
       <c r="AO12" s="1">
         <v>6</v>
       </c>
-      <c r="AP12" s="15"/>
-      <c r="AQ12" s="15"/>
-      <c r="AR12" s="15"/>
-      <c r="AS12" s="15"/>
-      <c r="AT12" s="15"/>
-      <c r="AU12" s="15"/>
-      <c r="AV12" s="15"/>
+      <c r="AP12" s="12"/>
+      <c r="AQ12" s="12"/>
+      <c r="AR12" s="12"/>
+      <c r="AS12" s="12"/>
+      <c r="AT12" s="12"/>
+      <c r="AU12" s="12"/>
+      <c r="AV12" s="12"/>
+      <c r="BJ12" s="19"/>
+      <c r="BK12" s="19"/>
+      <c r="BL12" s="19"/>
+      <c r="BM12" s="19"/>
+      <c r="BN12" s="19"/>
+      <c r="BO12" s="19"/>
+      <c r="BP12" s="19"/>
+      <c r="BQ12" s="19"/>
+      <c r="BR12" s="19"/>
+      <c r="BS12" s="19"/>
+      <c r="BT12" s="19"/>
+      <c r="BU12" s="19"/>
+      <c r="BV12" s="19"/>
+      <c r="BW12" s="19"/>
+      <c r="BX12" s="19"/>
+      <c r="BY12" s="19"/>
+      <c r="BZ12" s="19"/>
+      <c r="CA12" s="19"/>
+      <c r="CB12" s="19"/>
     </row>
-    <row r="13" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
@@ -1503,15 +1867,34 @@
       <c r="AO13" s="1">
         <v>8</v>
       </c>
-      <c r="AP13" s="15"/>
-      <c r="AQ13" s="15"/>
-      <c r="AR13" s="15"/>
-      <c r="AS13" s="14"/>
-      <c r="AT13" s="15"/>
-      <c r="AU13" s="15"/>
-      <c r="AV13" s="14"/>
+      <c r="AP13" s="12"/>
+      <c r="AQ13" s="12"/>
+      <c r="AR13" s="12"/>
+      <c r="AS13" s="11"/>
+      <c r="AT13" s="12"/>
+      <c r="AU13" s="12"/>
+      <c r="AV13" s="11"/>
+      <c r="BJ13" s="19"/>
+      <c r="BK13" s="19"/>
+      <c r="BL13" s="19"/>
+      <c r="BM13" s="19"/>
+      <c r="BN13" s="19"/>
+      <c r="BO13" s="19"/>
+      <c r="BP13" s="19"/>
+      <c r="BQ13" s="19"/>
+      <c r="BR13" s="19"/>
+      <c r="BS13" s="19"/>
+      <c r="BT13" s="19"/>
+      <c r="BU13" s="19"/>
+      <c r="BV13" s="19"/>
+      <c r="BW13" s="19"/>
+      <c r="BX13" s="19"/>
+      <c r="BY13" s="19"/>
+      <c r="BZ13" s="19"/>
+      <c r="CA13" s="19"/>
+      <c r="CB13" s="19"/>
     </row>
-    <row r="14" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="7" t="s">
         <v>10</v>
       </c>
@@ -1555,15 +1938,34 @@
       <c r="AM14" s="8"/>
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
-      <c r="AP14" s="15"/>
-      <c r="AQ14" s="15"/>
-      <c r="AR14" s="15"/>
-      <c r="AS14" s="15"/>
-      <c r="AT14" s="15"/>
-      <c r="AU14" s="15"/>
-      <c r="AV14" s="15"/>
+      <c r="AP14" s="12"/>
+      <c r="AQ14" s="12"/>
+      <c r="AR14" s="12"/>
+      <c r="AS14" s="12"/>
+      <c r="AT14" s="12"/>
+      <c r="AU14" s="12"/>
+      <c r="AV14" s="12"/>
+      <c r="BJ14" s="19"/>
+      <c r="BK14" s="19"/>
+      <c r="BL14" s="19"/>
+      <c r="BM14" s="19"/>
+      <c r="BN14" s="19"/>
+      <c r="BO14" s="19"/>
+      <c r="BP14" s="19"/>
+      <c r="BQ14" s="19"/>
+      <c r="BR14" s="19"/>
+      <c r="BS14" s="19"/>
+      <c r="BT14" s="19"/>
+      <c r="BU14" s="19"/>
+      <c r="BV14" s="19"/>
+      <c r="BW14" s="19"/>
+      <c r="BX14" s="19"/>
+      <c r="BY14" s="19"/>
+      <c r="BZ14" s="19"/>
+      <c r="CA14" s="19"/>
+      <c r="CB14" s="19"/>
     </row>
-    <row r="15" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="9" t="s">
         <v>11</v>
       </c>
@@ -1607,15 +2009,34 @@
       <c r="AM15" s="8"/>
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
-      <c r="AP15" s="15"/>
-      <c r="AQ15" s="15"/>
-      <c r="AR15" s="15"/>
-      <c r="AS15" s="15"/>
-      <c r="AT15" s="15"/>
-      <c r="AU15" s="15"/>
-      <c r="AV15" s="15"/>
+      <c r="AP15" s="12"/>
+      <c r="AQ15" s="12"/>
+      <c r="AR15" s="12"/>
+      <c r="AS15" s="12"/>
+      <c r="AT15" s="12"/>
+      <c r="AU15" s="12"/>
+      <c r="AV15" s="12"/>
+      <c r="BJ15" s="19"/>
+      <c r="BK15" s="19"/>
+      <c r="BL15" s="19"/>
+      <c r="BM15" s="19"/>
+      <c r="BN15" s="19"/>
+      <c r="BO15" s="19"/>
+      <c r="BP15" s="19"/>
+      <c r="BQ15" s="19"/>
+      <c r="BR15" s="19"/>
+      <c r="BS15" s="19"/>
+      <c r="BT15" s="19"/>
+      <c r="BU15" s="19"/>
+      <c r="BV15" s="19"/>
+      <c r="BW15" s="19"/>
+      <c r="BX15" s="19"/>
+      <c r="BY15" s="19"/>
+      <c r="BZ15" s="19"/>
+      <c r="CA15" s="19"/>
+      <c r="CB15" s="19"/>
     </row>
-    <row r="16" spans="1:61" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:81" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>12</v>
       </c>
@@ -1659,15 +2080,34 @@
       <c r="AM16" s="8"/>
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
-      <c r="AP16" s="15"/>
-      <c r="AQ16" s="15"/>
-      <c r="AR16" s="15"/>
-      <c r="AS16" s="15"/>
-      <c r="AT16" s="15"/>
-      <c r="AU16" s="15"/>
-      <c r="AV16" s="15"/>
+      <c r="AP16" s="12"/>
+      <c r="AQ16" s="12"/>
+      <c r="AR16" s="12"/>
+      <c r="AS16" s="12"/>
+      <c r="AT16" s="12"/>
+      <c r="AU16" s="12"/>
+      <c r="AV16" s="12"/>
+      <c r="BJ16" s="19"/>
+      <c r="BK16" s="19"/>
+      <c r="BL16" s="19"/>
+      <c r="BM16" s="19"/>
+      <c r="BN16" s="19"/>
+      <c r="BO16" s="19"/>
+      <c r="BP16" s="19"/>
+      <c r="BQ16" s="19"/>
+      <c r="BR16" s="19"/>
+      <c r="BS16" s="19"/>
+      <c r="BT16" s="19"/>
+      <c r="BU16" s="19"/>
+      <c r="BV16" s="19"/>
+      <c r="BW16" s="19"/>
+      <c r="BX16" s="19"/>
+      <c r="BY16" s="19"/>
+      <c r="BZ16" s="19"/>
+      <c r="CA16" s="19"/>
+      <c r="CB16" s="19"/>
     </row>
-    <row r="17" spans="1:48" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:80" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>13</v>
       </c>
@@ -1711,15 +2151,34 @@
       <c r="AM17" s="8"/>
       <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
-      <c r="AP17" s="15"/>
-      <c r="AQ17" s="15"/>
-      <c r="AR17" s="15"/>
-      <c r="AS17" s="15"/>
-      <c r="AT17" s="15"/>
-      <c r="AU17" s="15"/>
-      <c r="AV17" s="15"/>
+      <c r="AP17" s="12"/>
+      <c r="AQ17" s="12"/>
+      <c r="AR17" s="12"/>
+      <c r="AS17" s="12"/>
+      <c r="AT17" s="12"/>
+      <c r="AU17" s="12"/>
+      <c r="AV17" s="12"/>
+      <c r="BJ17" s="19"/>
+      <c r="BK17" s="19"/>
+      <c r="BL17" s="19"/>
+      <c r="BM17" s="19"/>
+      <c r="BN17" s="19"/>
+      <c r="BO17" s="19"/>
+      <c r="BP17" s="19"/>
+      <c r="BQ17" s="19"/>
+      <c r="BR17" s="19"/>
+      <c r="BS17" s="19"/>
+      <c r="BT17" s="19"/>
+      <c r="BU17" s="19"/>
+      <c r="BV17" s="19"/>
+      <c r="BW17" s="19"/>
+      <c r="BX17" s="19"/>
+      <c r="BY17" s="19"/>
+      <c r="BZ17" s="19"/>
+      <c r="CA17" s="19"/>
+      <c r="CB17" s="19"/>
     </row>
-    <row r="18" spans="1:48" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:80" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="9" t="s">
         <v>14</v>
       </c>
@@ -1763,16 +2222,59 @@
       <c r="AM18" s="8"/>
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
-      <c r="AP18" s="15"/>
-      <c r="AQ18" s="15"/>
-      <c r="AR18" s="15"/>
-      <c r="AS18" s="15"/>
-      <c r="AT18" s="15"/>
-      <c r="AU18" s="15"/>
-      <c r="AV18" s="15"/>
+      <c r="AP18" s="12"/>
+      <c r="AQ18" s="12"/>
+      <c r="AR18" s="12"/>
+      <c r="AS18" s="12"/>
+      <c r="AT18" s="12"/>
+      <c r="AU18" s="12"/>
+      <c r="AV18" s="12"/>
+      <c r="BJ18" s="19"/>
+      <c r="BK18" s="19"/>
+      <c r="BL18" s="19"/>
+      <c r="BM18" s="19"/>
+      <c r="BN18" s="19"/>
+      <c r="BO18" s="19"/>
+      <c r="BP18" s="19"/>
+      <c r="BQ18" s="19"/>
+      <c r="BR18" s="19"/>
+      <c r="BS18" s="19"/>
+      <c r="BT18" s="19"/>
+      <c r="BU18" s="19"/>
+      <c r="BV18" s="19"/>
+      <c r="BW18" s="19"/>
+      <c r="BX18" s="19"/>
+      <c r="BY18" s="19"/>
+      <c r="BZ18" s="19"/>
+      <c r="CA18" s="19"/>
+      <c r="CB18" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="32">
+    <mergeCell ref="BS1:BU1"/>
+    <mergeCell ref="BY1:CA1"/>
+    <mergeCell ref="CB1:CB3"/>
+    <mergeCell ref="CC1:CC3"/>
+    <mergeCell ref="BJ1:BL1"/>
+    <mergeCell ref="BM1:BO1"/>
+    <mergeCell ref="BP1:BR1"/>
+    <mergeCell ref="BV1:BX1"/>
+    <mergeCell ref="P1:S1"/>
+    <mergeCell ref="T1:T3"/>
+    <mergeCell ref="U1:U3"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="AJ1:AM1"/>
+    <mergeCell ref="AO1:AO3"/>
+    <mergeCell ref="AN1:AN3"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="Y1:AA1"/>
+    <mergeCell ref="AB1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
+    <mergeCell ref="AG1:AI1"/>
     <mergeCell ref="BD1:BG1"/>
     <mergeCell ref="BH1:BH3"/>
     <mergeCell ref="BI1:BI3"/>
@@ -1781,22 +2283,6 @@
     <mergeCell ref="AV1:AX1"/>
     <mergeCell ref="AY1:AZ1"/>
     <mergeCell ref="BA1:BC1"/>
-    <mergeCell ref="AJ1:AM1"/>
-    <mergeCell ref="AO1:AO3"/>
-    <mergeCell ref="AN1:AN3"/>
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="Y1:AA1"/>
-    <mergeCell ref="AB1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
-    <mergeCell ref="AG1:AI1"/>
-    <mergeCell ref="P1:S1"/>
-    <mergeCell ref="T1:T3"/>
-    <mergeCell ref="U1:U3"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:O1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>